<commit_message>
Signed-off-by: Mikhail Gerasimov <Gerasimov@dvugms.khv.ru>
</commit_message>
<xml_diff>
--- a/test/tel.xlsx
+++ b/test/tel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Автомобили с бробегом</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Хозяин</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>Гидра - Авто</t>
   </si>
   <si>
@@ -52,6 +55,15 @@
   </si>
   <si>
     <t>Михаил</t>
+  </si>
+  <si>
+    <t>Марина</t>
+  </si>
+  <si>
+    <t>Ж</t>
+  </si>
+  <si>
+    <t>Илья</t>
   </si>
 </sst>
 </file>
@@ -88,7 +100,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
@@ -393,27 +406,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="12" customWidth="1" style="2"/>
+    <col min="1" max="1" bestFit="1" width="12" customWidth="1" style="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2">
+      <c r="A1" s="3">
         <v>89859708676</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>89050397320</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -426,52 +439,140 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>84993907516</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>89128439000</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>89241086744</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>89241086745</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>89241086746</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>